<commit_message>
clutch mo na quibs
</commit_message>
<xml_diff>
--- a/backend/framework/packages/wcc.xlsx
+++ b/backend/framework/packages/wcc.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="34">
   <si>
     <t>Name</t>
   </si>
@@ -119,6 +119,18 @@
   </si>
   <si>
     <t>[tr_status]</t>
+  </si>
+  <si>
+    <t>[sd_date]</t>
+  </si>
+  <si>
+    <t>[sd_name]</t>
+  </si>
+  <si>
+    <t>[sd_vip]</t>
+  </si>
+  <si>
+    <t>[sd_invite]</t>
   </si>
 </sst>
 </file>
@@ -190,7 +202,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -201,6 +213,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -223,13 +241,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>10</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>1362022</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>1</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
+      <xdr:col>13</xdr:col>
       <xdr:colOff>22412</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>1</xdr:rowOff>
@@ -565,21 +583,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:V9"/>
+  <dimension ref="A1:T9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="6" width="20.7109375" customWidth="1"/>
-    <col min="8" max="12" width="20.7109375" customWidth="1"/>
-    <col min="14" max="16" width="20.7109375" customWidth="1"/>
-    <col min="18" max="22" width="20.7109375" customWidth="1"/>
+    <col min="1" max="5" width="20.7109375" customWidth="1"/>
+    <col min="7" max="11" width="20.7109375" customWidth="1"/>
+    <col min="13" max="15" width="20.7109375" customWidth="1"/>
+    <col min="17" max="18" width="20.7109375" customWidth="1"/>
+    <col min="19" max="20" width="20.7109375" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:22">
+    <row r="1" spans="1:20">
+      <c r="A1" s="4"/>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
@@ -599,10 +619,9 @@
       <c r="R1" s="4"/>
       <c r="S1" s="4"/>
       <c r="T1" s="4"/>
-      <c r="U1" s="4"/>
-      <c r="V1" s="4"/>
     </row>
-    <row r="2" spans="2:22">
+    <row r="2" spans="1:20">
+      <c r="A2" s="4"/>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
@@ -622,10 +641,9 @@
       <c r="R2" s="4"/>
       <c r="S2" s="4"/>
       <c r="T2" s="4"/>
-      <c r="U2" s="4"/>
-      <c r="V2" s="4"/>
     </row>
-    <row r="3" spans="2:22">
+    <row r="3" spans="1:20">
+      <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
@@ -645,10 +663,9 @@
       <c r="R3" s="4"/>
       <c r="S3" s="4"/>
       <c r="T3" s="4"/>
-      <c r="U3" s="4"/>
-      <c r="V3" s="4"/>
     </row>
-    <row r="4" spans="2:22">
+    <row r="4" spans="1:20">
+      <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
@@ -668,10 +685,9 @@
       <c r="R4" s="4"/>
       <c r="S4" s="4"/>
       <c r="T4" s="4"/>
-      <c r="U4" s="4"/>
-      <c r="V4" s="4"/>
     </row>
-    <row r="5" spans="2:22">
+    <row r="5" spans="1:20">
+      <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
@@ -691,10 +707,9 @@
       <c r="R5" s="4"/>
       <c r="S5" s="4"/>
       <c r="T5" s="4"/>
-      <c r="U5" s="4"/>
-      <c r="V5" s="4"/>
     </row>
-    <row r="6" spans="2:22">
+    <row r="6" spans="1:20">
+      <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
@@ -712,143 +727,147 @@
       <c r="P6" s="1"/>
       <c r="Q6" s="1"/>
       <c r="R6" s="1"/>
-      <c r="S6" s="1"/>
-      <c r="T6" s="1"/>
-      <c r="U6" s="1"/>
-      <c r="V6" s="1"/>
     </row>
-    <row r="7" spans="2:22">
-      <c r="B7" s="3" t="s">
+    <row r="7" spans="1:20">
+      <c r="A7" s="3" t="s">
         <v>3</v>
       </c>
+      <c r="B7" s="3"/>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="H7" s="3" t="s">
+      <c r="G7" s="3" t="s">
         <v>11</v>
       </c>
+      <c r="H7" s="3"/>
       <c r="I7" s="3"/>
       <c r="J7" s="3"/>
       <c r="K7" s="3"/>
-      <c r="L7" s="3"/>
-      <c r="N7" s="3" t="s">
+      <c r="M7" s="3" t="s">
         <v>13</v>
       </c>
+      <c r="N7" s="3"/>
       <c r="O7" s="3"/>
-      <c r="P7" s="3"/>
-      <c r="R7" s="3" t="s">
+      <c r="Q7" s="3" t="s">
         <v>16</v>
       </c>
+      <c r="R7" s="3"/>
       <c r="S7" s="3"/>
       <c r="T7" s="3"/>
-      <c r="U7" s="3"/>
-      <c r="V7" s="3"/>
     </row>
-    <row r="8" spans="2:22">
+    <row r="8" spans="1:20">
+      <c r="A8" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="B8" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C8" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="M8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="N8" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D8" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H8" s="2" t="s">
+      <c r="O8" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q8" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="I8" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="J8" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="K8" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="L8" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="N8" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="O8" s="2" t="s">
+      <c r="R8" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="P8" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="R8" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="S8" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="T8" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="U8" s="2" t="s">
+      <c r="S8" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="V8" s="2" t="s">
+      <c r="T8" s="6" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="2:22">
+    <row r="9" spans="1:20">
+      <c r="A9" t="s">
+        <v>25</v>
+      </c>
       <c r="B9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C9" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D9" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E9" t="s">
-        <v>28</v>
-      </c>
-      <c r="F9" t="s">
         <v>29</v>
       </c>
+      <c r="G9" t="s">
+        <v>20</v>
+      </c>
       <c r="H9" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I9" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="J9" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K9" t="s">
-        <v>23</v>
-      </c>
-      <c r="L9" t="s">
         <v>24</v>
       </c>
+      <c r="M9" t="s">
+        <v>17</v>
+      </c>
       <c r="N9" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="O9" t="s">
-        <v>18</v>
-      </c>
-      <c r="P9" t="s">
         <v>19</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>30</v>
+      </c>
+      <c r="R9" t="s">
+        <v>31</v>
+      </c>
+      <c r="S9" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="T9" s="5" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="B7:F7"/>
-    <mergeCell ref="H7:L7"/>
-    <mergeCell ref="N7:P7"/>
-    <mergeCell ref="R7:V7"/>
-    <mergeCell ref="B1:V5"/>
+    <mergeCell ref="A7:E7"/>
+    <mergeCell ref="G7:K7"/>
+    <mergeCell ref="M7:O7"/>
+    <mergeCell ref="Q7:T7"/>
+    <mergeCell ref="A1:T5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>